<commit_message>
Marked the completed tasks in the task document
</commit_message>
<xml_diff>
--- a/Documents/Tasks.xlsx
+++ b/Documents/Tasks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="27795" windowHeight="12840" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="27795" windowHeight="12840"/>
   </bookViews>
   <sheets>
     <sheet name="Task View" sheetId="1" r:id="rId1"/>
@@ -235,7 +235,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -250,13 +250,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -268,10 +280,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -289,16 +302,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -310,7 +322,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -326,22 +341,22 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B3:D40" totalsRowShown="0">
   <autoFilter ref="B3:D40"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Id" dataDxfId="0"/>
-    <tableColumn id="2" name="Narrative" dataDxfId="1"/>
-    <tableColumn id="3" name="Points" dataDxfId="5"/>
+    <tableColumn id="1" name="Id" dataDxfId="5"/>
+    <tableColumn id="2" name="Narrative" dataDxfId="4"/>
+    <tableColumn id="3" name="Points" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A3:A41" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A3:A41" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
   <autoFilter ref="A3:A41"/>
   <sortState ref="A4:A21">
     <sortCondition ref="A3:A41"/>
   </sortState>
   <tableColumns count="1">
-    <tableColumn id="1" name="Priority" dataDxfId="4"/>
+    <tableColumn id="1" name="Priority" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -636,8 +651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -662,12 +677,12 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
+      <c r="C6" s="7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
+      <c r="C7" s="7" t="s">
         <v>9</v>
       </c>
     </row>
@@ -891,7 +906,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Decreased the logo size.  Renamed a the new's to add's.
</commit_message>
<xml_diff>
--- a/Documents/Tasks.xlsx
+++ b/Documents/Tasks.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="76">
   <si>
     <t>Scrum Time 1.0 Tasks</t>
   </si>
@@ -229,13 +229,28 @@
   </si>
   <si>
     <t>self-contained installer</t>
+  </si>
+  <si>
+    <t>Make priority editable</t>
+  </si>
+  <si>
+    <t>Read-only points to editable combo w/ selection</t>
+  </si>
+  <si>
+    <t>Consistent naming of javascript/view/controller method</t>
+  </si>
+  <si>
+    <t>Decrease ScrumTime logo size</t>
+  </si>
+  <si>
+    <t>Priority solution</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -257,8 +272,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -270,8 +292,13 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -279,12 +306,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -303,9 +346,11 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Input" xfId="2" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="6">
@@ -649,16 +694,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:C54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="T32" sqref="T32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="5.7109375" customWidth="1"/>
-    <col min="3" max="3" width="45.140625" customWidth="1"/>
+    <col min="3" max="3" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
@@ -702,133 +747,133 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+      <c r="C11" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C12" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C13" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>52</v>
+      <c r="C18" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
-        <v>11</v>
+      <c r="C20" s="8" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
-        <v>5</v>
+      <c r="B21" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>14</v>
+      <c r="C24" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C30" t="s">
-        <v>22</v>
+      <c r="C30" s="8" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C31" t="s">
-        <v>20</v>
+      <c r="C31" s="8" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
-        <v>5</v>
+      <c r="B32" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>23</v>
+      <c r="C34" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
@@ -837,62 +882,87 @@
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C38" t="s">
-        <v>6</v>
+      <c r="C38" s="8" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C39" t="s">
-        <v>7</v>
+      <c r="B39" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>27</v>
+      <c r="C41" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C46" t="s">
-        <v>13</v>
+      <c r="B46" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>29</v>
+      <c r="C47" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C49" t="s">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>